<commit_message>
Add antTask.  Rename BlancoCalcWriter to BlancoCalcTransformer.  Abolished AbstractBlancoCalcWriter.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCommonsConstants.xlsx
+++ b/meta/program/BlancoCommonsConstants.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>定数定義書</t>
   </si>
@@ -201,6 +201,46 @@
   </si>
   <si>
     <t>STR_DELIMITER</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>PRODUCT_NAME</t>
+  </si>
+  <si>
+    <t>プロダクト名。英字で指定します。</t>
+  </si>
+  <si>
+    <t>PRODUCT_NAME_LOWER</t>
+  </si>
+  <si>
+    <t>プロダクト名の小文字版。英字で指定します。</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>"0.0.1"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>バージョン番号。</t>
+  </si>
+  <si>
+    <t>TARGET_SUBDIRECTORY</t>
+  </si>
+  <si>
+    <t>処理の過程で利用されるサブディレクトリ。</t>
+  </si>
+  <si>
+    <t>"BlancoCommons"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"blancocommons"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"/blancocommons"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -596,23 +636,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,7 +1037,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1041,7 +1081,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1069,7 +1109,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1230,19 +1270,19 @@
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E18" s="41" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="22"/>
@@ -1250,11 +1290,11 @@
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="23"/>
       <c r="G19"/>
       <c r="H19"/>
@@ -1264,16 +1304,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C20" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20"/>
@@ -1285,16 +1325,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21"/>
@@ -1306,16 +1346,16 @@
         <v>3</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E22" s="26" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22"/>
@@ -1327,16 +1367,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23"/>
@@ -1348,18 +1388,18 @@
         <v>5</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="28"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
@@ -1368,10 +1408,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
+      <c r="B25" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>30</v>
+      </c>
       <c r="F25" s="29"/>
       <c r="G25"/>
       <c r="H25"/>
@@ -1381,10 +1429,18 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
+      <c r="B26" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>29</v>
+      </c>
       <c r="F26" s="29"/>
       <c r="G26"/>
       <c r="H26"/>
@@ -1394,10 +1450,18 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
+      <c r="B27" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="F27" s="29"/>
       <c r="G27"/>
       <c r="H27"/>
@@ -1407,24 +1471,32 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
+      <c r="B28" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="F28" s="29"/>
       <c r="G28"/>
       <c r="H28"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="38">
+      <c r="A29" s="36">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
       <c r="G29"/>
       <c r="H29"/>
     </row>

</xml_diff>

<commit_message>
2.0.3: Now full maven buildable and compile as 1.8 (bitecode v.52)
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCommonsConstants.xlsx
+++ b/meta/program/BlancoCommonsConstants.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCommons/meta/program/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6EE6C8-8CBF-2449-B778-A0E9791C64AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="675" windowWidth="22860" windowHeight="8415" tabRatio="640"/>
+    <workbookView xWindow="460" yWindow="680" windowWidth="23680" windowHeight="14920" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -27,7 +33,17 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -219,10 +235,6 @@
     <t>VERSION</t>
   </si>
   <si>
-    <t>"0.0.1"</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>バージョン番号。</t>
   </si>
   <si>
@@ -241,13 +253,17 @@
   </si>
   <si>
     <t>"/blancocommons"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"2.0.3"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -728,6 +744,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1037,7 +1061,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1081,7 +1105,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1102,29 +1126,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="19">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1334,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>43</v>
@@ -1331,7 +1355,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>45</v>
@@ -1352,10 +1376,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22"/>
@@ -1367,16 +1391,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23"/>
@@ -1510,15 +1534,15 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>adjustConstValue</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>accessScope</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1532,20 +1556,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="8.125" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75">
+    <row r="1" spans="1:10" ht="19">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
[POI4] 2.1.2: apache poi 4.1.2 and xmlbeans 3.1.0 some times fails to evaluate fomula. So display current processing sheet and row and column, to avoid exception by modifying the sheet.(unfortunately, i cannot avoid this bug of them.)
</commit_message>
<xml_diff>
--- a/meta/program/BlancoCommonsConstants.xlsx
+++ b/meta/program/BlancoCommonsConstants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoCommons/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB2DF01-5C8E-6845-BDD6-AC602CFBB285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52A395-7866-8448-89E7-D047294F387C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="680" windowWidth="23680" windowHeight="14920" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,7 +256,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>"2.1.1"</t>
+    <t>"2.1.2"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1061,7 +1061,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1105,7 +1105,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>